<commit_message>
Author          : Prateek Kapoor Files Added     : PrateekKapoor.xlsx Description     : Updated Task Breakdown Sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prateek kapoor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11415" windowHeight="4605" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Name 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prateek-" sheetId="1" r:id="rId1"/>
     <sheet name="Name 2" sheetId="2" r:id="rId2"/>
     <sheet name="Name 3" sheetId="4" r:id="rId3"/>
     <sheet name="Name 4" sheetId="5" r:id="rId4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>Story ID</t>
   </si>
@@ -51,18 +51,12 @@
     <t>Story Estimate</t>
   </si>
   <si>
-    <t>SSDMS-098*</t>
-  </si>
-  <si>
     <t>Understanding the business</t>
   </si>
   <si>
     <t xml:space="preserve">Understanding the forward and backward linkages </t>
   </si>
   <si>
-    <t xml:space="preserve">Creating basic HTML and CSS Structure </t>
-  </si>
-  <si>
     <t xml:space="preserve">Implementing Angular JS for dynamic Behaviour  </t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>T-12</t>
   </si>
   <si>
-    <t>SSDMS-100*</t>
-  </si>
-  <si>
     <t>T-05</t>
   </si>
   <si>
@@ -138,28 +129,37 @@
     <t>Creating the HTML and CSS structure</t>
   </si>
   <si>
-    <t>Adding Functionality to get data from backend</t>
-  </si>
-  <si>
     <t>Unit Testing</t>
   </si>
   <si>
-    <t>SSDMS-101*</t>
-  </si>
-  <si>
-    <t>Creating the structure of AB home page using UI Grid</t>
-  </si>
-  <si>
-    <t>27 Hours</t>
-  </si>
-  <si>
-    <t>19 Hours</t>
-  </si>
-  <si>
     <t>Creating High-charts</t>
   </si>
   <si>
     <t>43 Hours</t>
+  </si>
+  <si>
+    <t>9 Hours</t>
+  </si>
+  <si>
+    <t>Creating basic HTML and CSS Structure - for page</t>
+  </si>
+  <si>
+    <t>Write SQL queries to fetch required data from tables in the DB</t>
+  </si>
+  <si>
+    <t>Receive sent response from SQL Queries in DTO</t>
+  </si>
+  <si>
+    <t>SSDMS-098*(Dashboard)</t>
+  </si>
+  <si>
+    <t>SSDMS-100* (Home Page TP)</t>
+  </si>
+  <si>
+    <t>SSDMS-101*(Home Page AB)</t>
+  </si>
+  <si>
+    <t>28 Hours</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,8 +196,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -220,11 +256,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -239,6 +343,61 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2819,15 +2978,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:XFD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="A16:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="67.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -2835,7 +2995,7 @@
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2858,428 +3018,471 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:G16" si="0">E4-F4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="7">
+        <v>7</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7">
+        <v>6</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7">
+        <v>14</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
+      <c r="F13" s="7"/>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2">
+    <row r="14" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="7">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G48" si="0">E4-F4</f>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2">
-        <v>6</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="2">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="XFD16">
+        <f>SUM(G16)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19">
+        <f>E17-F17</f>
+        <v>0.5</v>
+      </c>
+      <c r="XFD17">
+        <f>SUM(G17)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="19">
+        <v>5</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19">
+        <f>E18-F18</f>
+        <v>5</v>
+      </c>
+      <c r="XFD18">
+        <f>SUM(G18)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19">
+        <f>E19-F19</f>
+        <v>1</v>
+      </c>
+      <c r="XFD19">
+        <f>SUM(G19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="19">
+        <v>3</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19">
+        <f>E20-F20</f>
+        <v>3</v>
+      </c>
+      <c r="XFD20">
+        <f>SUM(G20)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="E21" s="19">
+        <v>6</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19">
+        <f>E21-F21</f>
+        <v>6</v>
+      </c>
+      <c r="XFD21">
+        <f>SUM(G21)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="19">
+        <v>5</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19">
+        <f>E22-F22</f>
+        <v>5</v>
+      </c>
+      <c r="XFD22">
+        <f>SUM(G22)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="19">
+        <v>6</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19">
+        <f>E23-F23</f>
+        <v>6</v>
+      </c>
+      <c r="XFD23">
+        <f>SUM(G23)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="19">
         <v>1</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19">
+        <f>E24-F24</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="XFD24">
+        <f>SUM(G24)</f>
         <v>1</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="25" spans="1:7 16384:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="2">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2">
-        <v>2</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="2">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="2">
-        <v>6</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="F25" s="19"/>
+      <c r="G25" s="19">
+        <f>E25-F25</f>
         <v>1</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
+      <c r="XFD25">
+        <f>SUM(G25)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19">
+        <f>E26-F26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3287,157 +3490,148 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1" t="s">
+        <f>E27-F27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26">
+        <f>E28-F28</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E29" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26">
+        <f>E29-F29</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="26">
+        <v>5</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26">
+        <f>E30-F30</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="26">
         <v>1</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26">
+        <f>E31-F31</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="2">
+    <row r="32" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="25">
         <v>1</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25">
+        <f>E32-F32</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="2">
-        <v>4</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="2">
-        <v>2</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="2">
-        <v>2</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="2">
-        <v>4</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="C33" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="26">
+        <v>1</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26">
+        <f>E33-F33</f>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="2">
-        <v>3</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="2">
-        <v>1</v>
-      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -3447,7 +3641,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2">
-        <f t="shared" si="0"/>
+        <f>E37-F37</f>
         <v>0</v>
       </c>
     </row>
@@ -3459,7 +3653,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
-        <f t="shared" si="0"/>
+        <f>E38-F38</f>
         <v>0</v>
       </c>
     </row>
@@ -3471,7 +3665,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
-        <f t="shared" si="0"/>
+        <f>E39-F39</f>
         <v>0</v>
       </c>
     </row>
@@ -3483,7 +3677,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2">
-        <f t="shared" si="0"/>
+        <f>E40-F40</f>
         <v>0</v>
       </c>
     </row>
@@ -3495,7 +3689,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2">
-        <f t="shared" si="0"/>
+        <f>E41-F41</f>
         <v>0</v>
       </c>
     </row>
@@ -3507,7 +3701,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" si="0"/>
+        <f>E42-F42</f>
         <v>0</v>
       </c>
     </row>
@@ -3519,7 +3713,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2">
-        <f t="shared" si="0"/>
+        <f>E43-F43</f>
         <v>0</v>
       </c>
     </row>
@@ -3531,7 +3725,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2">
-        <f t="shared" si="0"/>
+        <f>E44-F44</f>
         <v>0</v>
       </c>
     </row>
@@ -3543,7 +3737,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2">
-        <f t="shared" si="0"/>
+        <f>E45-F45</f>
         <v>0</v>
       </c>
     </row>
@@ -3555,7 +3749,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2">
-        <f t="shared" si="0"/>
+        <f>E46-F46</f>
         <v>0</v>
       </c>
     </row>
@@ -3567,7 +3761,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2">
-        <f t="shared" si="0"/>
+        <f>E47-F47</f>
         <v>0</v>
       </c>
     </row>
@@ -3579,11 +3773,16 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2">
-        <f t="shared" si="0"/>
+        <f>E48-F48</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A28:A35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Author            :Prateek Kapoor Files Modified    :PrateekKapoor.xlsx Description       :Excel Sheet updated after completing story SSDMS-101
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017.git\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Prateek and Arjita" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:XFD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,10 +1258,12 @@
       <c r="E30" s="17">
         <v>4</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="17">
+        <v>4</v>
+      </c>
       <c r="G30" s="17">
         <f>E30-F30</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1296,10 +1298,12 @@
       <c r="E32" s="16">
         <v>1</v>
       </c>
-      <c r="F32" s="16"/>
+      <c r="F32" s="16">
+        <v>1</v>
+      </c>
       <c r="G32" s="16">
         <f>E32-F32</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1314,10 +1318,12 @@
       <c r="E33" s="17">
         <v>1</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" s="17">
+        <v>1</v>
+      </c>
       <c r="G33" s="17">
         <f>E33-F33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author           : Prateek Kapoor Files Modified   : PrateekKapoor.xlsx Description      : Task number T-03 updated(Task completed) for story SSDMS-100
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:XFD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,14 +1012,16 @@
       <c r="E18" s="13">
         <v>4</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="13">
+        <v>1.5</v>
+      </c>
       <c r="G18" s="13">
         <f>E18-F18</f>
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="XFD18">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1259,11 +1261,11 @@
         <v>4</v>
       </c>
       <c r="F30" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G30" s="17">
         <f>E30-F30</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1299,11 +1301,11 @@
         <v>1</v>
       </c>
       <c r="F32" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G32" s="16">
         <f>E32-F32</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1319,11 +1321,11 @@
         <v>1</v>
       </c>
       <c r="F33" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G33" s="17">
         <f>E33-F33</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author           :Prateek Kapoor Files Modified   : PrateekKapoor.xlsx Description      :Added a new task to be completed
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Story ID</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>7.5 Hours</t>
+  </si>
+  <si>
+    <t>POC (SQL Queries and Backend)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t>Add data from database into the Angular UI Grid</t>
   </si>
 </sst>
 </file>
@@ -674,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:XFD48"/>
+  <dimension ref="A2:XFD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="A16:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,9 +698,10 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -713,8 +723,11 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>25</v>
       </c>
@@ -737,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
       <c r="B4" s="2"/>
       <c r="C4" s="14" t="s">
@@ -753,11 +766,11 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:G16" si="0">E4-F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G4:G26" si="0">E4-F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
       <c r="B5" s="2"/>
       <c r="C5" s="14" t="s">
@@ -777,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="2"/>
       <c r="C6" s="14" t="s">
@@ -795,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="2"/>
       <c r="C7" s="14" t="s">
@@ -813,7 +826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="2"/>
       <c r="C8" s="14" t="s">
@@ -831,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="2"/>
       <c r="C9" s="14" t="s">
@@ -849,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="2"/>
       <c r="C10" s="14" t="s">
@@ -867,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="2"/>
       <c r="C11" s="14" t="s">
@@ -885,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="2"/>
       <c r="C12" s="14" t="s">
@@ -903,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="2"/>
       <c r="C13" s="14" t="s">
@@ -921,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="2"/>
       <c r="C14" s="14" t="s">
@@ -939,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -948,7 +961,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>26</v>
       </c>
@@ -972,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="XFD16">
-        <f t="shared" ref="XFD16:XFD25" si="1">SUM(G16)</f>
+        <f t="shared" ref="XFD16:XFD26" si="1">SUM(G16)</f>
         <v>0</v>
       </c>
     </row>
@@ -992,7 +1005,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="13">
-        <f>E17-F17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="XFD17">
@@ -1016,7 +1029,7 @@
         <v>1.5</v>
       </c>
       <c r="G18" s="13">
-        <f>E18-F18</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="XFD18">
@@ -1040,7 +1053,7 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="13">
-        <f>E19-F19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="XFD19">
@@ -1060,14 +1073,16 @@
       <c r="E20" s="13">
         <v>2</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="F20" s="13">
+        <v>0.5</v>
+      </c>
       <c r="G20" s="13">
-        <f>E20-F20</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
       <c r="XFD20">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="21" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1082,14 +1097,16 @@
       <c r="E21" s="13">
         <v>5</v>
       </c>
-      <c r="F21" s="13"/>
+      <c r="F21" s="13">
+        <v>5</v>
+      </c>
       <c r="G21" s="13">
-        <f>E21-F21</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="XFD21">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1104,14 +1121,16 @@
       <c r="E22" s="13">
         <v>4</v>
       </c>
-      <c r="F22" s="13"/>
+      <c r="F22" s="13">
+        <v>4</v>
+      </c>
       <c r="G22" s="13">
-        <f>E22-F22</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="XFD22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1126,14 +1145,16 @@
       <c r="E23" s="13">
         <v>2</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="13">
+        <v>2</v>
+      </c>
       <c r="G23" s="13">
-        <f>E23-F23</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="XFD23">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
@@ -1143,36 +1164,38 @@
         <v>10</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E24" s="13">
-        <v>1</v>
-      </c>
-      <c r="F24" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="F24" s="13">
+        <v>1</v>
+      </c>
       <c r="G24" s="13">
-        <f>E24-F24</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="XFD24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7 16384:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
       <c r="B25" s="2"/>
       <c r="C25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E25" s="13">
         <v>1</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13">
-        <f>E25-F25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="XFD25">
@@ -1180,62 +1203,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+    <row r="26" spans="1:7 16384:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="13">
+        <v>1</v>
+      </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13">
-        <f>E26-F26</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="XFD26">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2">
+      <c r="C27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="13">
+        <v>2</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13">
         <f>E27-F27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2">
+        <f>E28-F28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B29" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="E28" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F28" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="G28" s="17">
-        <f>E28-F28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="E29" s="17">
         <v>0.5</v>
@@ -1252,78 +1285,78 @@
       <c r="A30" s="25"/>
       <c r="B30" s="2"/>
       <c r="C30" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E30" s="17">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="F30" s="17">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G30" s="17">
         <f>E30-F30</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="2"/>
       <c r="C31" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E31" s="17">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="F31" s="17">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G31" s="17">
         <f>E31-F31</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="2"/>
       <c r="C32" s="17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="16">
-        <v>1</v>
-      </c>
-      <c r="F32" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="G32" s="16">
+        <v>32</v>
+      </c>
+      <c r="E32" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="17">
         <f>E32-F32</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="2"/>
       <c r="C33" s="17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="17">
-        <v>1</v>
-      </c>
-      <c r="F33" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="G33" s="17">
+        <v>22</v>
+      </c>
+      <c r="E33" s="16">
+        <v>1</v>
+      </c>
+      <c r="F33" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="16">
         <f>E33-F33</f>
         <v>0.5</v>
       </c>
@@ -1331,29 +1364,43 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
+      <c r="C34" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="17">
+        <v>1</v>
+      </c>
+      <c r="F34" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="17">
+        <f>E34-F34</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="2"/>
       <c r="C35" s="17"/>
       <c r="D35" s="16"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="17">
+        <f>SUM(G16:G27)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -1362,10 +1409,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <f t="shared" ref="G37:G48" si="2">E37-F37</f>
-        <v>0</v>
-      </c>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -1375,7 +1419,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G38:G49" si="2">E38-F38</f>
         <v>0</v>
       </c>
     </row>
@@ -1499,11 +1543,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="A16:A26"/>
     <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A29:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author             :Prateek Kapoor Files Modified     :PrateekKapoor.xlsx Description        :New task added in story SSDMS-101 as task T-06
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t>Story ID</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>IN DEV</t>
+  </si>
+  <si>
+    <t>NG-Include to include files into master HTML</t>
   </si>
 </sst>
 </file>
@@ -389,6 +392,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,9 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:XFD52"/>
+  <dimension ref="A2:XFD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,12 +743,12 @@
       <c r="H2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -774,7 +777,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2"/>
       <c r="C4" s="10" t="s">
         <v>17</v>
@@ -798,7 +801,7 @@
       <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2"/>
       <c r="C5" s="10" t="s">
         <v>16</v>
@@ -822,7 +825,7 @@
       <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2"/>
       <c r="C6" s="10" t="s">
         <v>15</v>
@@ -844,7 +847,7 @@
       <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
         <v>14</v>
@@ -866,7 +869,7 @@
       <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2"/>
       <c r="C8" s="10" t="s">
         <v>13</v>
@@ -888,7 +891,7 @@
       <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="2"/>
       <c r="C9" s="10" t="s">
         <v>12</v>
@@ -910,7 +913,7 @@
       <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10" t="s">
         <v>11</v>
@@ -932,7 +935,7 @@
       <c r="I10" s="28"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="2"/>
       <c r="C11" s="10" t="s">
         <v>10</v>
@@ -954,7 +957,7 @@
       <c r="I11" s="28"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2"/>
       <c r="C12" s="10" t="s">
         <v>9</v>
@@ -976,7 +979,7 @@
       <c r="I12" s="28"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="2"/>
       <c r="C13" s="10" t="s">
         <v>19</v>
@@ -998,7 +1001,7 @@
       <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="2"/>
       <c r="C14" s="10" t="s">
         <v>20</v>
@@ -1053,7 +1056,7 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -1086,7 +1089,7 @@
       </c>
     </row>
     <row r="19" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2"/>
       <c r="C19" s="9" t="s">
         <v>17</v>
@@ -1114,7 +1117,7 @@
       </c>
     </row>
     <row r="20" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2"/>
       <c r="C20" s="9" t="s">
         <v>16</v>
@@ -1142,7 +1145,7 @@
       </c>
     </row>
     <row r="21" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="2"/>
       <c r="C21" s="9" t="s">
         <v>15</v>
@@ -1170,7 +1173,7 @@
       </c>
     </row>
     <row r="22" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="2"/>
       <c r="C22" s="9" t="s">
         <v>21</v>
@@ -1198,7 +1201,7 @@
       </c>
     </row>
     <row r="23" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="2"/>
       <c r="C23" s="9" t="s">
         <v>13</v>
@@ -1226,7 +1229,7 @@
       </c>
     </row>
     <row r="24" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="2"/>
       <c r="C24" s="9" t="s">
         <v>12</v>
@@ -1254,7 +1257,7 @@
       </c>
     </row>
     <row r="25" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="2"/>
       <c r="C25" s="9" t="s">
         <v>11</v>
@@ -1282,7 +1285,7 @@
       </c>
     </row>
     <row r="26" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="2"/>
       <c r="C26" s="9" t="s">
         <v>10</v>
@@ -1310,7 +1313,7 @@
       </c>
     </row>
     <row r="27" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="2"/>
       <c r="C27" s="9" t="s">
         <v>9</v>
@@ -1336,7 +1339,7 @@
       </c>
     </row>
     <row r="28" spans="1:9 16384:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="2"/>
       <c r="C28" s="9" t="s">
         <v>19</v>
@@ -1408,7 +1411,7 @@
       <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="13" t="s">
@@ -1438,7 +1441,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="2"/>
       <c r="C33" s="13" t="s">
         <v>17</v>
@@ -1453,7 +1456,7 @@
         <v>0.5</v>
       </c>
       <c r="G33" s="13">
-        <f t="shared" ref="G33:G37" si="2">E33-F33</f>
+        <f t="shared" ref="G33:G38" si="2">E33-F33</f>
         <v>0</v>
       </c>
       <c r="H33" s="13" t="s">
@@ -1462,7 +1465,7 @@
       <c r="I33" s="30"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="2"/>
       <c r="C34" s="13" t="s">
         <v>16</v>
@@ -1486,7 +1489,7 @@
       <c r="I34" s="30"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="2"/>
       <c r="C35" s="13" t="s">
         <v>15</v>
@@ -1510,7 +1513,7 @@
       <c r="I35" s="30"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="2"/>
       <c r="C36" s="13" t="s">
         <v>21</v>
@@ -1534,40 +1537,52 @@
       <c r="I36" s="30"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="2"/>
       <c r="C37" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="13">
-        <v>1</v>
-      </c>
-      <c r="F37" s="13">
-        <v>0.5</v>
+        <v>52</v>
+      </c>
+      <c r="E37" s="12">
+        <v>2</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0</v>
       </c>
       <c r="G37" s="13">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H37" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="30"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="13">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="13">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H38" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I37" s="30"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="10">
-        <f>SUM(G32:G37)</f>
-        <v>3</v>
-      </c>
+      <c r="I38" s="30"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
@@ -1576,28 +1591,28 @@
       <c r="D39" s="15"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
+      <c r="G39" s="10">
+        <f>SUM(G32:G38)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
       <c r="E40" s="14"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2">
-        <f t="shared" ref="G41:G52" si="3">E41-F41</f>
-        <v>0</v>
-      </c>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -1607,7 +1622,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G42:G53" si="3">E42-F42</f>
         <v>0</v>
       </c>
     </row>
@@ -1731,14 +1746,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A18:A28"/>
     <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="A32:A40"/>
     <mergeCell ref="I3:I14"/>
     <mergeCell ref="I18:I29"/>
-    <mergeCell ref="I32:I37"/>
+    <mergeCell ref="I32:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author             :Prateek Kapoor Files Modified     :PrateekKapoor.xlsx Description        :new task added in story SSDMS-101 T-06
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:XFD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
       <c r="A38" s="26"/>
       <c r="B38" s="2"/>
       <c r="C38" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Author      :Arjita for Prateek Files Added :PrateekKapoor.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>Story ID</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>IN DEV</t>
-  </si>
-  <si>
-    <t>NG-Include to include files into master HTML</t>
   </si>
 </sst>
 </file>
@@ -699,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:XFD53"/>
+  <dimension ref="A2:XFD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C38"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,8 +1241,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>47</v>
@@ -1253,7 +1249,7 @@
       <c r="I24" s="29"/>
       <c r="XFD24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
@@ -1324,18 +1320,20 @@
       <c r="E27" s="9">
         <v>1</v>
       </c>
-      <c r="F27" s="9"/>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
       <c r="G27" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I27" s="29"/>
       <c r="XFD27">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9 16384:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1350,7 +1348,9 @@
       <c r="E28" s="9">
         <v>1</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
       <c r="G28" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1377,14 +1377,14 @@
         <v>2</v>
       </c>
       <c r="F29" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I29" s="29"/>
     </row>
@@ -1397,7 +1397,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="20">
         <f>SUM(G18:G29)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1456,7 +1456,7 @@
         <v>0.5</v>
       </c>
       <c r="G33" s="13">
-        <f t="shared" ref="G33:G38" si="2">E33-F33</f>
+        <f t="shared" ref="G33:G37" si="2">E33-F33</f>
         <v>0</v>
       </c>
       <c r="H33" s="13" t="s">
@@ -1543,76 +1543,64 @@
         <v>13</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="12">
-        <v>2</v>
-      </c>
-      <c r="F37" s="12">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E37" s="13">
+        <v>1</v>
+      </c>
+      <c r="F37" s="13">
+        <v>0.5</v>
       </c>
       <c r="G37" s="13">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I37" s="30"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="13">
-        <v>1</v>
-      </c>
-      <c r="F38" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G38" s="13">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38" s="30"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="10">
+        <f>SUM(G32:G37)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="2"/>
       <c r="C39" s="14"/>
       <c r="D39" s="15"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="10">
-        <f>SUM(G32:G38)</f>
-        <v>5</v>
-      </c>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="15"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="14"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2">
+        <f t="shared" ref="G41:G52" si="3">E41-F41</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -1622,7 +1610,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" ref="G42:G53" si="3">E42-F42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1746,26 +1734,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A18:A28"/>
     <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="A32:A39"/>
     <mergeCell ref="I3:I14"/>
     <mergeCell ref="I18:I29"/>
-    <mergeCell ref="I32:I38"/>
+    <mergeCell ref="I32:I37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author         :Arjita for Prateek Files Modified :PrateekKapoor.xlsx Description    :Task Updated
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:XFD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,10 +833,12 @@
       <c r="E6" s="6">
         <v>4</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
       <c r="G6" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>49</v>
@@ -855,7 +857,9 @@
       <c r="E7" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -877,10 +881,12 @@
       <c r="E8" s="6">
         <v>2</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>49</v>
@@ -919,12 +925,12 @@
         <v>34</v>
       </c>
       <c r="E10" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>49</v>
@@ -943,10 +949,12 @@
       <c r="E11" s="6">
         <v>1</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>49</v>
@@ -963,12 +971,12 @@
         <v>37</v>
       </c>
       <c r="E12" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>49</v>
@@ -1028,7 +1036,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="21">
         <f>SUM(G3:G14)</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -1126,11 +1134,11 @@
         <v>4</v>
       </c>
       <c r="F20" s="9">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>47</v>
@@ -1138,7 +1146,7 @@
       <c r="I20" s="29"/>
       <c r="XFD20">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
@@ -1182,11 +1190,11 @@
         <v>2</v>
       </c>
       <c r="F22" s="9">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>47</v>
@@ -1194,7 +1202,7 @@
       <c r="I22" s="29"/>
       <c r="XFD22">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
@@ -1241,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>47</v>
@@ -1249,7 +1257,7 @@
       <c r="I24" s="29"/>
       <c r="XFD24">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
@@ -1290,14 +1298,14 @@
         <v>46</v>
       </c>
       <c r="E26" s="9">
+        <v>4</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
-      </c>
-      <c r="F26" s="9">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>48</v>
@@ -1305,7 +1313,7 @@
       <c r="I26" s="29"/>
       <c r="XFD26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
@@ -1397,7 +1405,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="20">
         <f>SUM(G18:G29)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1477,11 +1485,11 @@
         <v>4</v>
       </c>
       <c r="F34" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G34" s="13">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>47</v>
@@ -1525,11 +1533,11 @@
         <v>1</v>
       </c>
       <c r="F36" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G36" s="13">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>47</v>
@@ -1549,11 +1557,11 @@
         <v>1</v>
       </c>
       <c r="F37" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G37" s="13">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>47</v>
@@ -1569,7 +1577,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="10">
         <f>SUM(G32:G37)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author         :Prateek Files Modified :PrateekKapoor.xlsx Description    :Task Updated in story SSDMS-99
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
+++ b/TeamDetails/TasksBreakDown/PrateekKapoor.xlsx
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:XFD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,11 +858,11 @@
         <v>4</v>
       </c>
       <c r="F7" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>49</v>
@@ -1036,7 +1036,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="21">
         <f>SUM(G3:G14)</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H15" s="2"/>
     </row>

</xml_diff>